<commit_message>
cambio de telefono a lista de tipo sangre
</commit_message>
<xml_diff>
--- a/WebFPRTest/obj/Release/net6.0/PubTmp/Out/wwwroot/Archivos/FormatoCargaMasiva.xlsx
+++ b/WebFPRTest/obj/Release/net6.0/PubTmp/Out/wwwroot/Archivos/FormatoCargaMasiva.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desarrollos\WebFPRTest\WebFPRTest\wwwroot\Archivos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AlucarD-LAP\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7B84B28-1364-43B9-B99A-7CB1582F6DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31170" yWindow="2310" windowWidth="21600" windowHeight="11835" xr2:uid="{013104E6-93CE-4948-A6F8-95E76ECDD659}"/>
+    <workbookView xWindow="31170" yWindow="2310" windowWidth="21600" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,12 +33,63 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Victor Felipa Tejada</author>
+    <author>AlucarD-LAP</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{1E33B604-DE51-4AA3-B766-85B61F18DA88}">
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>FPR:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+1: DNI
+2: Carnet Extranjeria
+3: Pasaporte</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="1" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>AlucarD-LAP:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Correo de WorldRugby</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -49,7 +99,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>FPR:</t>
+          <t>AlucarD-LAP:</t>
         </r>
         <r>
           <rPr>
@@ -59,9 +109,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-1: DNI
-2: Carnet Extranjeria
-3: Pasaporte</t>
+4: MASCULINO
+5: FEMENINO</t>
         </r>
       </text>
     </comment>
@@ -70,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Nombres</t>
   </si>
@@ -96,48 +145,77 @@
     <t>Correo</t>
   </si>
   <si>
-    <t>Mendoza</t>
-  </si>
-  <si>
-    <t>Regalado</t>
-  </si>
-  <si>
-    <t>Ricardo</t>
-  </si>
-  <si>
-    <t>09450945</t>
-  </si>
-  <si>
-    <t>951951951</t>
-  </si>
-  <si>
-    <t>ricardo@gmail.com</t>
-  </si>
-  <si>
-    <t>Chavez</t>
-  </si>
-  <si>
-    <t>Noriega</t>
-  </si>
-  <si>
-    <t>Jorge</t>
-  </si>
-  <si>
-    <t>09784512</t>
-  </si>
-  <si>
-    <t>987987987</t>
-  </si>
-  <si>
-    <t>jorge@gmail.com</t>
+    <t>Felipa</t>
+  </si>
+  <si>
+    <t>45586417</t>
+  </si>
+  <si>
+    <t>Pilar</t>
+  </si>
+  <si>
+    <t>pilar@gmail.com</t>
+  </si>
+  <si>
+    <t>Martinez</t>
+  </si>
+  <si>
+    <t>Tejada</t>
+  </si>
+  <si>
+    <t>04587121</t>
+  </si>
+  <si>
+    <t>987456123</t>
+  </si>
+  <si>
+    <t>Sexo</t>
+  </si>
+  <si>
+    <t>Victor</t>
+  </si>
+  <si>
+    <t>961261925</t>
+  </si>
+  <si>
+    <t>vdanfel@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -156,14 +234,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -187,11 +257,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -506,11 +577,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB32644-29F2-4FFF-82FA-B20DF9B1A175}">
-  <dimension ref="A1:H3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,7 +593,7 @@
     <col min="8" max="8" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -547,13 +618,16 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>10</v>
@@ -562,36 +636,39 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2">
+        <v>36526</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2">
-        <v>32131</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C3" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F3" s="2">
-        <v>32643</v>
+        <v>32507</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
@@ -599,19 +676,72 @@
       <c r="H3" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="I3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H10" s="3"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H13" s="3"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="H19" s="3"/>
+    </row>
+    <row r="26" spans="8:11" x14ac:dyDescent="0.25">
+      <c r="K26" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{DBEBC04B-DD26-419C-8523-413253EDAAB2}">
+  <dataValidations count="2">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
       <formula1>1</formula1>
       <formula2>3</formula2>
     </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I1048576">
+      <formula1>4</formula1>
+      <formula2>5</formula2>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" xr:uid="{8C121E92-D00E-4A64-B5E3-A50FABAC0A81}"/>
-    <hyperlink ref="H3" r:id="rId2" xr:uid="{984B6390-2075-49BA-B040-288EFF5F762C}"/>
+    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="H3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
+  <legacyDrawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>